<commit_message>
AI conversion and adjustment
</commit_message>
<xml_diff>
--- a/r/calculate_marks.xlsx
+++ b/r/calculate_marks.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3654A5C0-A831-463D-877A-1374B82042E2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="1185" yWindow="3930" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -117,7 +124,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -429,11 +436,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,7 +599,7 @@
         <v>9</v>
       </c>
       <c r="C18">
-        <f t="shared" ref="C18:C21" si="1">LN(B18+1)</f>
+        <f t="shared" ref="C18:C23" si="1">LN(B18+1)</f>
         <v>2.3025850929940459</v>
       </c>
     </row>
@@ -630,6 +637,24 @@
       <c r="C21">
         <f t="shared" si="1"/>
         <v>6.3117348091529148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>23000</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>10.043292972227004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>10000000</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>16.118095750958314</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>